<commit_message>
Added materials to BOM
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jordan_Robarts\Spinning_Jig_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jordan_Robarts\Spinning_Jig_Project\Cardiac-Organ\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -483,13 +483,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="3" builtinId="4"/>
@@ -794,10 +794,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="23"/>
       <c r="C1" s="8" t="s">
         <v>8</v>
       </c>
@@ -1567,7 +1567,7 @@
       <c r="J3" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="23" t="s">
+      <c r="K3" s="21" t="s">
         <v>44</v>
       </c>
       <c r="L3" s="11"/>

</xml_diff>